<commit_message>
30-11-2019 : Minor Bug Fix ->User Management
</commit_message>
<xml_diff>
--- a/upload_template/LeaveBalance_Upload.xlsx
+++ b/upload_template/LeaveBalance_Upload.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +451,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="D2" s="1">
         <v>20005890</v>
@@ -471,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="D3" s="1">
         <v>20005890</v>
@@ -491,7 +491,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="D4" s="1">
         <v>20005890</v>
@@ -511,7 +511,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="D5" s="1">
         <v>20005890</v>

</xml_diff>